<commit_message>
first push dataset statistics summary
</commit_message>
<xml_diff>
--- a/Report/project description/ML_techniques_list.xlsx
+++ b/Report/project description/ML_techniques_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Deakin/Projects/Dean_Summer_Project_2025/Out-of-distribution-data-fitting/Report/project description/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460A2BF6-C0CF-594D-B8B0-54A97758A006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73489164-4A10-6E44-A4EC-9654AA19CAA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="3" xr2:uid="{6F2F4567-F782-CF4C-A67E-9B64C68C02AD}"/>
   </bookViews>
@@ -2739,8 +2739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4496F88-B485-484B-945C-BFB9552D104E}">
   <dimension ref="A1:E205"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.2"/>

</xml_diff>